<commit_message>
Finished graph and report
</commit_message>
<xml_diff>
--- a/project1/Graph.xlsx
+++ b/project1/Graph.xlsx
@@ -1,31 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mustafa/Desktop/NMSU/Courses/CS 474/Projects/Fall 2024/Project1/Skeleton_Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominik\Desktop\CS Folder\CS474_OS\cs474\project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882AA6EC-BCD4-F042-90AE-E5439D61DA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5D35E1-6ACB-450D-B883-0C1B2A4FACB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16420" xr2:uid="{867B545B-DBDD-874D-9C3F-1FC2BE1AB2D3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{867B545B-DBDD-874D-9C3F-1FC2BE1AB2D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$A$2:$A$10</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$C$2:$C$10</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$A$2:$A$10</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">Sheet1!$C$2:$C$10</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -61,7 +51,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -273,31 +263,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.50491610412498822</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.26303984412362186</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.13285272994023786</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.1005669740783728</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>9.7728822809889412E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>9.3239811623644073E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>9.4582655124671386E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>9.6412998292786198E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1516,17 +1506,17 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.375" customWidth="1"/>
+    <col min="3" max="3" width="22.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16.5" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1537,94 +1527,112 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1" t="e">
+      <c r="B2" s="2">
+        <v>2.5907710000000002</v>
+      </c>
+      <c r="C2" s="1">
         <f>B2/$B$2</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1" t="e">
+      <c r="B3" s="2">
+        <v>1.308122</v>
+      </c>
+      <c r="C3" s="1">
         <f t="shared" ref="C3:C10" si="0">B3/$B$2</f>
-        <v>#DIV/0!</v>
+        <v>0.50491610412498822</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>4</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1" t="e">
+      <c r="B4" s="2">
+        <v>0.68147599999999997</v>
+      </c>
+      <c r="C4" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.26303984412362186</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>8</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="1" t="e">
+      <c r="B5" s="2">
+        <v>0.34419100000000002</v>
+      </c>
+      <c r="C5" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.13285272994023786</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>16</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="1" t="e">
+      <c r="B6" s="2">
+        <v>0.260546</v>
+      </c>
+      <c r="C6" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.1005669740783728</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>32</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="1" t="e">
+      <c r="B7" s="2">
+        <v>0.253193</v>
+      </c>
+      <c r="C7" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>9.7728822809889412E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>64</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="1" t="e">
+      <c r="B8" s="2">
+        <v>0.241563</v>
+      </c>
+      <c r="C8" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>9.3239811623644073E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>128</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="1" t="e">
+      <c r="B9" s="2">
+        <v>0.24504200000000001</v>
+      </c>
+      <c r="C9" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>9.4582655124671386E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>256</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="1" t="e">
+      <c r="B10" s="2">
+        <v>0.24978400000000001</v>
+      </c>
+      <c r="C10" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>9.6412998292786198E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>